<commit_message>
update path for results
</commit_message>
<xml_diff>
--- a/003__shift_planning/src/main/resources/tables.xlsx
+++ b/003__shift_planning/src/main/resources/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\portafolio\003__shift_planning\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCBD830-20F1-4256-B56E-FB7A1F28EDC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6E1DA9-2753-4FC2-ABFE-BFB3B85E9333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-210" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="employees" sheetId="1" r:id="rId1"/>
@@ -468,10 +468,14 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B6"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -486,8 +490,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <f>48*4</f>
-        <v>192</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -495,8 +498,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B6" si="0">48*4</f>
-        <v>192</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -504,8 +506,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
-        <v>192</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -513,8 +514,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>192</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -522,8 +522,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>192</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -537,11 +536,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -588,7 +588,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +639,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="A2" sqref="A2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>